<commit_message>
Added thumbnails (journal cover) for Rural21 missed ones
</commit_message>
<xml_diff>
--- a/landlibrary/importers/Rural21/20170202 - Rural21 - Land Library Metadata_EN_13-16.xlsx
+++ b/landlibrary/importers/Rural21/20170202 - Rural21 - Land Library Metadata_EN_13-16.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="25596" windowHeight="14484" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="20170202 - Rural21 - Land Libra" sheetId="1" r:id="rId1"/>
     <sheet name="notes" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="330"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="503">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1188" uniqueCount="507">
   <si>
     <t>Abstract/Description</t>
   </si>
@@ -1669,6 +1669,18 @@
   </si>
   <si>
     <t>Rural21-Vol:13-Nr:2/2006-Article:20</t>
+  </si>
+  <si>
+    <t>private://feeds/Rural21_2009-04_en.jpg</t>
+  </si>
+  <si>
+    <t>private://feeds/Rural21_2008-01_en.jpg</t>
+  </si>
+  <si>
+    <t>private://feeds/Rural21_2007-01_en.jpg</t>
+  </si>
+  <si>
+    <t>private://feeds/Rural21_2006-02_en.jpg</t>
   </si>
 </sst>
 </file>
@@ -2066,9 +2078,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C43" sqref="C43:C62"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S43" sqref="S43:S62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.796875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2090,7 +2102,7 @@
     <col min="16" max="16" width="22.5" style="1" customWidth="1"/>
     <col min="17" max="17" width="56.796875" style="10" customWidth="1"/>
     <col min="18" max="18" width="35" style="1" customWidth="1"/>
-    <col min="19" max="19" width="10.796875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="31.59765625" style="1" customWidth="1"/>
     <col min="20" max="20" width="21.5" style="1" customWidth="1"/>
     <col min="21" max="16384" width="10.796875" style="1"/>
   </cols>
@@ -2210,6 +2222,9 @@
       <c r="R2" s="8" t="s">
         <v>70</v>
       </c>
+      <c r="S2" s="1" t="s">
+        <v>503</v>
+      </c>
       <c r="T2" s="1" t="s">
         <v>425</v>
       </c>
@@ -2266,6 +2281,9 @@
       <c r="R3" s="8" t="s">
         <v>72</v>
       </c>
+      <c r="S3" s="1" t="s">
+        <v>503</v>
+      </c>
       <c r="T3" s="1" t="s">
         <v>425</v>
       </c>
@@ -2323,6 +2341,9 @@
       <c r="R4" s="8" t="s">
         <v>75</v>
       </c>
+      <c r="S4" s="1" t="s">
+        <v>503</v>
+      </c>
       <c r="T4" s="1" t="s">
         <v>425</v>
       </c>
@@ -2382,6 +2403,9 @@
       <c r="R5" s="8" t="s">
         <v>83</v>
       </c>
+      <c r="S5" s="1" t="s">
+        <v>503</v>
+      </c>
       <c r="T5" s="1" t="s">
         <v>425</v>
       </c>
@@ -2438,6 +2462,9 @@
       <c r="R6" s="8" t="s">
         <v>80</v>
       </c>
+      <c r="S6" s="1" t="s">
+        <v>503</v>
+      </c>
       <c r="T6" s="1" t="s">
         <v>425</v>
       </c>
@@ -2495,6 +2522,9 @@
       <c r="R7" s="8" t="s">
         <v>86</v>
       </c>
+      <c r="S7" s="1" t="s">
+        <v>503</v>
+      </c>
       <c r="T7" s="1" t="s">
         <v>425</v>
       </c>
@@ -2554,6 +2584,9 @@
       <c r="R8" s="8" t="s">
         <v>89</v>
       </c>
+      <c r="S8" s="1" t="s">
+        <v>503</v>
+      </c>
       <c r="T8" s="1" t="s">
         <v>425</v>
       </c>
@@ -2613,6 +2646,9 @@
       <c r="R9" s="8" t="s">
         <v>94</v>
       </c>
+      <c r="S9" s="1" t="s">
+        <v>503</v>
+      </c>
       <c r="T9" s="1" t="s">
         <v>425</v>
       </c>
@@ -2671,6 +2707,9 @@
       </c>
       <c r="R10" s="8" t="s">
         <v>98</v>
+      </c>
+      <c r="S10" s="1" t="s">
+        <v>503</v>
       </c>
       <c r="T10" s="1" t="s">
         <v>425</v>
@@ -2729,6 +2768,9 @@
       <c r="R11" s="8" t="s">
         <v>101</v>
       </c>
+      <c r="S11" s="1" t="s">
+        <v>503</v>
+      </c>
       <c r="T11" s="1" t="s">
         <v>425</v>
       </c>
@@ -2779,6 +2821,9 @@
       <c r="R12" s="8" t="s">
         <v>103</v>
       </c>
+      <c r="S12" s="1" t="s">
+        <v>503</v>
+      </c>
       <c r="T12" s="1" t="s">
         <v>425</v>
       </c>
@@ -2838,6 +2883,9 @@
       <c r="R13" s="8" t="s">
         <v>108</v>
       </c>
+      <c r="S13" s="1" t="s">
+        <v>504</v>
+      </c>
       <c r="T13" s="1" t="s">
         <v>425</v>
       </c>
@@ -2892,6 +2940,9 @@
       <c r="R14" s="8" t="s">
         <v>112</v>
       </c>
+      <c r="S14" s="1" t="s">
+        <v>504</v>
+      </c>
       <c r="T14" s="1" t="s">
         <v>425</v>
       </c>
@@ -2948,6 +2999,9 @@
       <c r="R15" s="8" t="s">
         <v>115</v>
       </c>
+      <c r="S15" s="1" t="s">
+        <v>504</v>
+      </c>
       <c r="T15" s="1" t="s">
         <v>425</v>
       </c>
@@ -3004,6 +3058,9 @@
       <c r="R16" s="8" t="s">
         <v>118</v>
       </c>
+      <c r="S16" s="1" t="s">
+        <v>504</v>
+      </c>
       <c r="T16" s="1" t="s">
         <v>425</v>
       </c>
@@ -3060,6 +3117,9 @@
       <c r="R17" s="8" t="s">
         <v>121</v>
       </c>
+      <c r="S17" s="1" t="s">
+        <v>504</v>
+      </c>
       <c r="T17" s="1" t="s">
         <v>425</v>
       </c>
@@ -3110,6 +3170,9 @@
       <c r="R18" s="8" t="s">
         <v>124</v>
       </c>
+      <c r="S18" s="1" t="s">
+        <v>504</v>
+      </c>
       <c r="T18" s="1" t="s">
         <v>425</v>
       </c>
@@ -3169,6 +3232,9 @@
       <c r="R19" s="8" t="s">
         <v>127</v>
       </c>
+      <c r="S19" s="1" t="s">
+        <v>504</v>
+      </c>
       <c r="T19" s="1" t="s">
         <v>425</v>
       </c>
@@ -3228,6 +3294,9 @@
       <c r="R20" s="8" t="s">
         <v>130</v>
       </c>
+      <c r="S20" s="1" t="s">
+        <v>504</v>
+      </c>
       <c r="T20" s="1" t="s">
         <v>425</v>
       </c>
@@ -3283,6 +3352,9 @@
       </c>
       <c r="R21" s="8" t="s">
         <v>132</v>
+      </c>
+      <c r="S21" s="1" t="s">
+        <v>504</v>
       </c>
       <c r="T21" s="1" t="s">
         <v>425</v>
@@ -3341,6 +3413,9 @@
       <c r="R22" s="8" t="s">
         <v>136</v>
       </c>
+      <c r="S22" s="1" t="s">
+        <v>504</v>
+      </c>
       <c r="T22" s="1" t="s">
         <v>425</v>
       </c>
@@ -3394,6 +3469,9 @@
       <c r="R23" s="8" t="s">
         <v>139</v>
       </c>
+      <c r="S23" s="1" t="s">
+        <v>504</v>
+      </c>
       <c r="T23" s="1" t="s">
         <v>425</v>
       </c>
@@ -3453,6 +3531,9 @@
       <c r="R24" s="8" t="s">
         <v>141</v>
       </c>
+      <c r="S24" s="1" t="s">
+        <v>505</v>
+      </c>
       <c r="T24" s="1" t="s">
         <v>425</v>
       </c>
@@ -3509,6 +3590,9 @@
       <c r="R25" s="8" t="s">
         <v>146</v>
       </c>
+      <c r="S25" s="1" t="s">
+        <v>505</v>
+      </c>
       <c r="T25" s="1" t="s">
         <v>425</v>
       </c>
@@ -3566,6 +3650,9 @@
       <c r="R26" s="8" t="s">
         <v>149</v>
       </c>
+      <c r="S26" s="1" t="s">
+        <v>505</v>
+      </c>
       <c r="T26" s="1" t="s">
         <v>425</v>
       </c>
@@ -3622,6 +3709,9 @@
       <c r="R27" s="8" t="s">
         <v>151</v>
       </c>
+      <c r="S27" s="1" t="s">
+        <v>505</v>
+      </c>
       <c r="T27" s="1" t="s">
         <v>425</v>
       </c>
@@ -3679,6 +3769,9 @@
       <c r="R28" s="8" t="s">
         <v>155</v>
       </c>
+      <c r="S28" s="1" t="s">
+        <v>505</v>
+      </c>
       <c r="T28" s="1" t="s">
         <v>425</v>
       </c>
@@ -3735,6 +3828,9 @@
       <c r="R29" s="8" t="s">
         <v>158</v>
       </c>
+      <c r="S29" s="1" t="s">
+        <v>505</v>
+      </c>
       <c r="T29" s="1" t="s">
         <v>425</v>
       </c>
@@ -3794,6 +3890,9 @@
       <c r="R30" s="8" t="s">
         <v>162</v>
       </c>
+      <c r="S30" s="1" t="s">
+        <v>505</v>
+      </c>
       <c r="T30" s="1" t="s">
         <v>425</v>
       </c>
@@ -3853,6 +3952,9 @@
       <c r="R31" s="8" t="s">
         <v>165</v>
       </c>
+      <c r="S31" s="1" t="s">
+        <v>505</v>
+      </c>
       <c r="T31" s="1" t="s">
         <v>425</v>
       </c>
@@ -3907,6 +4009,9 @@
       <c r="R32" s="8" t="s">
         <v>168</v>
       </c>
+      <c r="S32" s="1" t="s">
+        <v>505</v>
+      </c>
       <c r="T32" s="1" t="s">
         <v>425</v>
       </c>
@@ -3960,6 +4065,9 @@
       <c r="R33" s="8" t="s">
         <v>171</v>
       </c>
+      <c r="S33" s="1" t="s">
+        <v>505</v>
+      </c>
       <c r="T33" s="1" t="s">
         <v>425</v>
       </c>
@@ -4019,6 +4127,9 @@
       <c r="R34" s="8" t="s">
         <v>174</v>
       </c>
+      <c r="S34" s="1" t="s">
+        <v>505</v>
+      </c>
       <c r="T34" s="1" t="s">
         <v>425</v>
       </c>
@@ -4076,6 +4187,9 @@
       <c r="R35" s="8" t="s">
         <v>177</v>
       </c>
+      <c r="S35" s="1" t="s">
+        <v>505</v>
+      </c>
       <c r="T35" s="1" t="s">
         <v>425</v>
       </c>
@@ -4133,6 +4247,9 @@
       <c r="R36" s="8" t="s">
         <v>180</v>
       </c>
+      <c r="S36" s="1" t="s">
+        <v>505</v>
+      </c>
       <c r="T36" s="1" t="s">
         <v>425</v>
       </c>
@@ -4189,6 +4306,9 @@
       <c r="R37" s="8" t="s">
         <v>183</v>
       </c>
+      <c r="S37" s="1" t="s">
+        <v>505</v>
+      </c>
       <c r="T37" s="1" t="s">
         <v>425</v>
       </c>
@@ -4246,6 +4366,9 @@
       <c r="R38" s="8" t="s">
         <v>186</v>
       </c>
+      <c r="S38" s="1" t="s">
+        <v>505</v>
+      </c>
       <c r="T38" s="1" t="s">
         <v>425</v>
       </c>
@@ -4305,6 +4428,9 @@
       <c r="R39" s="8" t="s">
         <v>190</v>
       </c>
+      <c r="S39" s="1" t="s">
+        <v>505</v>
+      </c>
       <c r="T39" s="1" t="s">
         <v>425</v>
       </c>
@@ -4361,6 +4487,9 @@
       <c r="R40" s="8" t="s">
         <v>193</v>
       </c>
+      <c r="S40" s="1" t="s">
+        <v>505</v>
+      </c>
       <c r="T40" s="1" t="s">
         <v>425</v>
       </c>
@@ -4420,6 +4549,9 @@
       <c r="R41" s="8" t="s">
         <v>196</v>
       </c>
+      <c r="S41" s="1" t="s">
+        <v>505</v>
+      </c>
       <c r="T41" s="1" t="s">
         <v>425</v>
       </c>
@@ -4479,6 +4611,9 @@
       <c r="R42" s="8" t="s">
         <v>199</v>
       </c>
+      <c r="S42" s="1" t="s">
+        <v>505</v>
+      </c>
       <c r="T42" s="1" t="s">
         <v>425</v>
       </c>
@@ -4538,6 +4673,9 @@
       <c r="R43" s="8" t="s">
         <v>203</v>
       </c>
+      <c r="S43" s="1" t="s">
+        <v>506</v>
+      </c>
       <c r="T43" s="1" t="s">
         <v>425</v>
       </c>
@@ -4594,6 +4732,9 @@
       <c r="R44" s="8" t="s">
         <v>206</v>
       </c>
+      <c r="S44" s="1" t="s">
+        <v>506</v>
+      </c>
       <c r="T44" s="1" t="s">
         <v>425</v>
       </c>
@@ -4650,6 +4791,9 @@
       <c r="R45" s="8" t="s">
         <v>209</v>
       </c>
+      <c r="S45" s="1" t="s">
+        <v>506</v>
+      </c>
       <c r="T45" s="1" t="s">
         <v>425</v>
       </c>
@@ -4707,6 +4851,9 @@
       <c r="R46" s="8" t="s">
         <v>212</v>
       </c>
+      <c r="S46" s="1" t="s">
+        <v>506</v>
+      </c>
       <c r="T46" s="1" t="s">
         <v>425</v>
       </c>
@@ -4766,6 +4913,9 @@
       <c r="R47" s="8" t="s">
         <v>215</v>
       </c>
+      <c r="S47" s="1" t="s">
+        <v>506</v>
+      </c>
       <c r="T47" s="1" t="s">
         <v>425</v>
       </c>
@@ -4825,6 +4975,9 @@
       <c r="R48" s="8" t="s">
         <v>218</v>
       </c>
+      <c r="S48" s="1" t="s">
+        <v>506</v>
+      </c>
       <c r="T48" s="1" t="s">
         <v>425</v>
       </c>
@@ -4881,6 +5034,9 @@
       <c r="R49" s="8" t="s">
         <v>221</v>
       </c>
+      <c r="S49" s="1" t="s">
+        <v>506</v>
+      </c>
       <c r="T49" s="1" t="s">
         <v>425</v>
       </c>
@@ -4940,6 +5096,9 @@
       <c r="R50" s="8" t="s">
         <v>225</v>
       </c>
+      <c r="S50" s="1" t="s">
+        <v>506</v>
+      </c>
       <c r="T50" s="1" t="s">
         <v>425</v>
       </c>
@@ -4992,6 +5151,9 @@
       </c>
       <c r="R51" s="8" t="s">
         <v>228</v>
+      </c>
+      <c r="S51" s="1" t="s">
+        <v>506</v>
       </c>
       <c r="T51" s="1" t="s">
         <v>425</v>
@@ -5049,6 +5211,9 @@
       <c r="R52" s="8" t="s">
         <v>230</v>
       </c>
+      <c r="S52" s="1" t="s">
+        <v>506</v>
+      </c>
       <c r="T52" s="1" t="s">
         <v>425</v>
       </c>
@@ -5105,6 +5270,9 @@
       <c r="R53" s="8" t="s">
         <v>232</v>
       </c>
+      <c r="S53" s="1" t="s">
+        <v>506</v>
+      </c>
       <c r="T53" s="1" t="s">
         <v>425</v>
       </c>
@@ -5158,6 +5326,9 @@
       <c r="R54" s="8" t="s">
         <v>237</v>
       </c>
+      <c r="S54" s="1" t="s">
+        <v>506</v>
+      </c>
       <c r="T54" s="1" t="s">
         <v>425</v>
       </c>
@@ -5211,6 +5382,9 @@
       <c r="R55" s="8" t="s">
         <v>240</v>
       </c>
+      <c r="S55" s="1" t="s">
+        <v>506</v>
+      </c>
       <c r="T55" s="1" t="s">
         <v>425</v>
       </c>
@@ -5264,6 +5438,9 @@
       <c r="R56" s="8" t="s">
         <v>243</v>
       </c>
+      <c r="S56" s="1" t="s">
+        <v>506</v>
+      </c>
       <c r="T56" s="1" t="s">
         <v>425</v>
       </c>
@@ -5323,6 +5500,9 @@
       <c r="R57" s="8" t="s">
         <v>245</v>
       </c>
+      <c r="S57" s="1" t="s">
+        <v>506</v>
+      </c>
       <c r="T57" s="1" t="s">
         <v>425</v>
       </c>
@@ -5382,6 +5562,9 @@
       <c r="R58" s="8" t="s">
         <v>249</v>
       </c>
+      <c r="S58" s="1" t="s">
+        <v>506</v>
+      </c>
       <c r="T58" s="1" t="s">
         <v>425</v>
       </c>
@@ -5438,6 +5621,9 @@
       <c r="R59" s="8" t="s">
         <v>252</v>
       </c>
+      <c r="S59" s="1" t="s">
+        <v>506</v>
+      </c>
       <c r="T59" s="1" t="s">
         <v>425</v>
       </c>
@@ -5497,6 +5683,9 @@
       <c r="R60" s="8" t="s">
         <v>256</v>
       </c>
+      <c r="S60" s="1" t="s">
+        <v>506</v>
+      </c>
       <c r="T60" s="1" t="s">
         <v>425</v>
       </c>
@@ -5556,6 +5745,9 @@
       <c r="R61" s="8" t="s">
         <v>260</v>
       </c>
+      <c r="S61" s="1" t="s">
+        <v>506</v>
+      </c>
       <c r="T61" s="1" t="s">
         <v>425</v>
       </c>
@@ -5612,6 +5804,9 @@
       </c>
       <c r="R62" s="8" t="s">
         <v>264</v>
+      </c>
+      <c r="S62" s="1" t="s">
+        <v>506</v>
       </c>
       <c r="T62" s="1" t="s">
         <v>425</v>

</xml_diff>